<commit_message>
Update Android Task Tracked Documents.xlsx
</commit_message>
<xml_diff>
--- a/Android Task Tracked Documents.xlsx
+++ b/Android Task Tracked Documents.xlsx
@@ -188,6 +188,7 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -816,12 +817,6 @@
   </cellStyleXfs>
   <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -834,9 +829,229 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -846,62 +1061,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,181 +1082,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1227,14 +1228,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
@@ -1299,20 +1305,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>219075</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
@@ -1377,20 +1388,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
@@ -1455,20 +1471,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
@@ -1533,20 +1554,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
@@ -1611,20 +1637,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>219075</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
@@ -1689,20 +1720,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
@@ -1767,20 +1803,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
@@ -1845,20 +1886,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
@@ -1923,20 +1969,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>219075</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
@@ -2001,20 +2052,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>679076</xdr:colOff>
+          <xdr:colOff>676275</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>186018</xdr:rowOff>
+          <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="219075"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>676275</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
@@ -2079,20 +2135,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>685800</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
@@ -2157,20 +2218,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>11205</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>179294</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
@@ -2235,20 +2301,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
@@ -2313,20 +2384,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>6723</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>366993</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="219075"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
@@ -2391,20 +2467,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
@@ -2469,20 +2550,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
@@ -2547,20 +2633,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>685800</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
@@ -2625,20 +2716,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>1680</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>379319</xdr:rowOff>
+          <xdr:rowOff>381000</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>685800</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
@@ -2703,20 +2799,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>16248</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>366993</xdr:rowOff>
+          <xdr:rowOff>371475</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="219075"/>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -2781,20 +2882,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
@@ -2859,20 +2965,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>685800</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
@@ -2937,20 +3048,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
@@ -3015,20 +3131,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>9</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
@@ -3093,20 +3214,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1049" name="Check Box 25" hidden="1">
@@ -3171,20 +3297,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1050" name="Check Box 26" hidden="1">
@@ -3249,20 +3380,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>1680</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>379319</xdr:rowOff>
+          <xdr:rowOff>381000</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>685800</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1051" name="Check Box 27" hidden="1">
@@ -3327,20 +3463,25 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="683559" cy="220756"/>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1052" name="Check Box 28" hidden="1">
@@ -3405,7 +3546,7 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -3807,294 +3948,294 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="82"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="18"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="16" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="16" t="s">
+      <c r="I7" s="10"/>
+      <c r="J7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="17"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="19" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="19" t="s">
+      <c r="I8" s="13"/>
+      <c r="J8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="20"/>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="16" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="16" t="s">
+      <c r="I9" s="11"/>
+      <c r="J9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="18"/>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19" t="s">
+      <c r="E10" s="13"/>
+      <c r="F10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16" t="s">
+      <c r="E11" s="10"/>
+      <c r="F11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="18"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19" t="s">
+      <c r="E12" s="13"/>
+      <c r="F12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="19" t="s">
+      <c r="G12" s="13"/>
+      <c r="H12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="16" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="16" t="s">
+      <c r="E13" s="10"/>
+      <c r="F13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="16" t="s">
+      <c r="G13" s="10"/>
+      <c r="H13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="18"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="19" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="20"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="15" spans="2:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="24"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4103,14 +4244,15 @@
     <mergeCell ref="D2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId3" name="Check Box 1">
+            <control shapeId="1025" r:id="rId4" name="Check Box 1">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4132,7 +4274,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId4" name="Check Box 2">
+            <control shapeId="1026" r:id="rId5" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4154,7 +4296,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1027" r:id="rId5" name="Check Box 3">
+            <control shapeId="1027" r:id="rId6" name="Check Box 3">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4176,7 +4318,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1028" r:id="rId6" name="Check Box 4">
+            <control shapeId="1028" r:id="rId7" name="Check Box 4">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4198,7 +4340,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId7" name="Check Box 5">
+            <control shapeId="1029" r:id="rId8" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4220,7 +4362,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId8" name="Check Box 6">
+            <control shapeId="1030" r:id="rId9" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4242,7 +4384,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1031" r:id="rId9" name="Check Box 7">
+            <control shapeId="1031" r:id="rId10" name="Check Box 7">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4264,7 +4406,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId10" name="Check Box 8">
+            <control shapeId="1032" r:id="rId11" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4286,7 +4428,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId11" name="Check Box 9">
+            <control shapeId="1033" r:id="rId12" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4308,7 +4450,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId12" name="Check Box 10">
+            <control shapeId="1034" r:id="rId13" name="Check Box 10">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4330,7 +4472,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId13" name="Check Box 11">
+            <control shapeId="1035" r:id="rId14" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4352,7 +4494,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId14" name="Check Box 12">
+            <control shapeId="1036" r:id="rId15" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4374,7 +4516,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId15" name="Check Box 13">
+            <control shapeId="1037" r:id="rId16" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4396,7 +4538,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId16" name="Check Box 14">
+            <control shapeId="1038" r:id="rId17" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4418,7 +4560,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId17" name="Check Box 15">
+            <control shapeId="1039" r:id="rId18" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4440,7 +4582,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId18" name="Check Box 16">
+            <control shapeId="1040" r:id="rId19" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4462,7 +4604,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId19" name="Check Box 17">
+            <control shapeId="1041" r:id="rId20" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4484,7 +4626,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId20" name="Check Box 18">
+            <control shapeId="1042" r:id="rId21" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4506,7 +4648,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId21" name="Check Box 19">
+            <control shapeId="1043" r:id="rId22" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4528,7 +4670,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1044" r:id="rId22" name="Check Box 20">
+            <control shapeId="1044" r:id="rId23" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4550,7 +4692,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1045" r:id="rId23" name="Check Box 21">
+            <control shapeId="1045" r:id="rId24" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4572,7 +4714,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId24" name="Check Box 22">
+            <control shapeId="1046" r:id="rId25" name="Check Box 22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4594,7 +4736,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1047" r:id="rId25" name="Check Box 23">
+            <control shapeId="1047" r:id="rId26" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4616,7 +4758,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId26" name="Check Box 24">
+            <control shapeId="1048" r:id="rId27" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4638,7 +4780,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId27" name="Check Box 25">
+            <control shapeId="1049" r:id="rId28" name="Check Box 25">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4660,7 +4802,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId28" name="Check Box 26">
+            <control shapeId="1050" r:id="rId29" name="Check Box 26">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4682,7 +4824,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1051" r:id="rId29" name="Check Box 27">
+            <control shapeId="1051" r:id="rId30" name="Check Box 27">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4704,7 +4846,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1052" r:id="rId30" name="Check Box 28">
+            <control shapeId="1052" r:id="rId31" name="Check Box 28">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4726,7 +4868,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1053" r:id="rId31" name="Check Box 29">
+            <control shapeId="1053" r:id="rId32" name="Check Box 29">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4757,7 +4899,7 @@
   <dimension ref="B1:G46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4772,473 +4914,473 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="86"/>
+      <c r="D2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="41" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="85"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="72"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="53"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="91" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="61"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="50"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="66"/>
-      <c r="C6" s="74" t="s">
+      <c r="B6" s="92"/>
+      <c r="C6" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="74"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="61"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="78"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="65"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="88"/>
+      <c r="C8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="79"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="66"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="35" t="s">
+      <c r="B9" s="88"/>
+      <c r="C9" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="79"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="66"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="35" t="s">
+      <c r="B10" s="88"/>
+      <c r="C10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="79"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="66"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="35" t="s">
+      <c r="B11" s="88"/>
+      <c r="C11" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="79"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="66"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="35" t="s">
+      <c r="B12" s="88"/>
+      <c r="C12" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="79"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="66"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
-      <c r="C13" s="35" t="s">
+      <c r="B13" s="88"/>
+      <c r="C13" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="79"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="66"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
-      <c r="C14" s="35" t="s">
+      <c r="B14" s="88"/>
+      <c r="C14" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="79"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="66"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="35" t="s">
+      <c r="B15" s="88"/>
+      <c r="C15" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="48"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="79"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="66"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
-      <c r="C16" s="35" t="s">
+      <c r="B16" s="88"/>
+      <c r="C16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="79"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="66"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="32"/>
-      <c r="C17" s="35" t="s">
+      <c r="B17" s="88"/>
+      <c r="C17" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="79"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="66"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="33"/>
-      <c r="C18" s="36" t="s">
+      <c r="B18" s="89"/>
+      <c r="C18" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="36"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="80"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="67"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="51"/>
-      <c r="C20" s="38" t="s">
+      <c r="B20" s="90"/>
+      <c r="C20" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="81"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="68"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="51"/>
-      <c r="C21" s="38" t="s">
+      <c r="B21" s="90"/>
+      <c r="C21" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="81"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="68"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="51"/>
-      <c r="C22" s="38" t="s">
+      <c r="B22" s="90"/>
+      <c r="C22" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="81"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="68"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="51"/>
-      <c r="C23" s="38" t="s">
+      <c r="B23" s="90"/>
+      <c r="C23" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="81"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="68"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="51"/>
-      <c r="C24" s="38" t="s">
+      <c r="B24" s="90"/>
+      <c r="C24" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="81"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="68"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="51"/>
-      <c r="C25" s="38" t="s">
+      <c r="B25" s="90"/>
+      <c r="C25" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="81"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="68"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="51"/>
-      <c r="C26" s="38" t="s">
+      <c r="B26" s="90"/>
+      <c r="C26" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="81"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="68"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="51"/>
-      <c r="C27" s="38" t="s">
+      <c r="B27" s="90"/>
+      <c r="C27" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="81"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="68"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="51"/>
-      <c r="C28" s="38" t="s">
+      <c r="B28" s="90"/>
+      <c r="C28" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="81"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="68"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="51"/>
-      <c r="C29" s="38" t="s">
+      <c r="B29" s="90"/>
+      <c r="C29" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="81"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="68"/>
     </row>
     <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="51"/>
-      <c r="C30" s="39" t="s">
+      <c r="B30" s="90"/>
+      <c r="C30" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="71"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="73"/>
-      <c r="G30" s="82"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="69"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="83"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="70"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="32"/>
-      <c r="C32" s="35" t="s">
+      <c r="B32" s="88"/>
+      <c r="C32" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="48"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="79"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="66"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="32"/>
-      <c r="C33" s="35" t="s">
+      <c r="B33" s="88"/>
+      <c r="C33" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="48"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="79"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="66"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="32"/>
-      <c r="C34" s="35" t="s">
+      <c r="B34" s="88"/>
+      <c r="C34" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D34" s="48"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="79"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="66"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="32"/>
-      <c r="C35" s="35" t="s">
+      <c r="B35" s="88"/>
+      <c r="C35" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="79"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="66"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="32"/>
-      <c r="C36" s="35" t="s">
+      <c r="B36" s="88"/>
+      <c r="C36" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="48"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="79"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="66"/>
     </row>
     <row r="37" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="33"/>
-      <c r="C37" s="40" t="s">
+      <c r="B37" s="89"/>
+      <c r="C37" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="36"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C38" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="67"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="80"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="67"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="51"/>
-      <c r="C39" s="38" t="s">
+      <c r="B39" s="90"/>
+      <c r="C39" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="81"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="68"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="51"/>
-      <c r="C40" s="38" t="s">
+      <c r="B40" s="90"/>
+      <c r="C40" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="70"/>
-      <c r="G40" s="81"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="68"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="51"/>
-      <c r="C41" s="38" t="s">
+      <c r="B41" s="90"/>
+      <c r="C41" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="81"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="68"/>
     </row>
     <row r="42" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="51"/>
-      <c r="C42" s="41" t="s">
+      <c r="B42" s="90"/>
+      <c r="C42" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="71"/>
-      <c r="E42" s="72"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="82"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="69"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="34" t="s">
+      <c r="C43" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="83"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="70"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="32"/>
-      <c r="C44" s="35" t="s">
+      <c r="B44" s="88"/>
+      <c r="C44" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="48"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="79"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="66"/>
     </row>
     <row r="45" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="33"/>
-      <c r="C45" s="40" t="s">
+      <c r="B45" s="89"/>
+      <c r="C45" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="30"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="84"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="71"/>
     </row>
     <row r="46" spans="2:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="25"/>
-      <c r="C46" s="86"/>
-      <c r="D46" s="87" t="s">
+      <c r="B46" s="18"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="E46" s="88"/>
-      <c r="F46" s="89">
+      <c r="E46" s="84"/>
+      <c r="F46" s="74">
         <v>43605</v>
       </c>
     </row>

</xml_diff>